<commit_message>
Auto stash before merge of "master" and "origin/elias"
</commit_message>
<xml_diff>
--- a/Nana&Rene/testProductos.xlsx
+++ b/Nana&Rene/testProductos.xlsx
@@ -29,19 +29,19 @@
     <t>torta</t>
   </si>
   <si>
-    <t>leche,harina,huevos,vainilla,</t>
+    <t>huevos,vainilla,leche,harina,</t>
   </si>
   <si>
     <t>kuchen</t>
   </si>
   <si>
-    <t>manzana,huevos,harina,</t>
+    <t>harina,manzana,huevos,</t>
   </si>
   <si>
     <t>queque</t>
   </si>
   <si>
-    <t>vainilla,harina,huevos,</t>
+    <t>huevos,vainilla,harina,</t>
   </si>
   <si>
     <t>tartaleta</t>
@@ -53,7 +53,7 @@
     <t>pie de limon</t>
   </si>
   <si>
-    <t>merengue,harina,crema, limon, huevos,</t>
+    <t>crema,harina, limon, huevos,merengue,</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Actualizacion de resumen pedidos pagina principal
</commit_message>
<xml_diff>
--- a/Nana&Rene/testProductos.xlsx
+++ b/Nana&Rene/testProductos.xlsx
@@ -29,19 +29,19 @@
     <t>torta</t>
   </si>
   <si>
-    <t>vainilla,harina,leche,huevos,</t>
+    <t>huevos,harina,vainilla,leche,</t>
   </si>
   <si>
     <t>kuchen</t>
   </si>
   <si>
-    <t>manzana,huevos,harina,</t>
+    <t>huevos,harina,manzana,</t>
   </si>
   <si>
     <t>queque</t>
   </si>
   <si>
-    <t>huevos,harina,vainilla,</t>
+    <t>huevos,vainilla,harina,</t>
   </si>
   <si>
     <t>tartaleta durazno</t>
@@ -53,7 +53,7 @@
     <t>pie de limon</t>
   </si>
   <si>
-    <t>merengue,crema, huevos, limon,harina,</t>
+    <t>harina, huevos, limon,merengue,crema,</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Actualizar tablas al editar
</commit_message>
<xml_diff>
--- a/Nana&Rene/testProductos.xlsx
+++ b/Nana&Rene/testProductos.xlsx
@@ -29,19 +29,19 @@
     <t>torta</t>
   </si>
   <si>
-    <t>huevos,harina,vainilla,leche,</t>
+    <t>leche,harina,huevos,vainilla,</t>
   </si>
   <si>
     <t>kuchen</t>
   </si>
   <si>
-    <t>huevos,harina,manzana,</t>
+    <t>manzana,huevos,harina,</t>
   </si>
   <si>
     <t>queque</t>
   </si>
   <si>
-    <t>huevos,vainilla,harina,</t>
+    <t>vainilla,harina,huevos,</t>
   </si>
   <si>
     <t>tartaleta durazno</t>
@@ -53,7 +53,7 @@
     <t>pie de limon</t>
   </si>
   <si>
-    <t>harina, huevos, limon,merengue,crema,</t>
+    <t>merengue,harina,crema, limon, huevos,</t>
   </si>
 </sst>
 </file>

</xml_diff>